<commit_message>
empiezp de calculo num maquinarias
</commit_message>
<xml_diff>
--- a/corte relleno.xlsx
+++ b/corte relleno.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>diagrama masas</t>
   </si>
@@ -42,7 +43,7 @@
     <t>/100*100</t>
   </si>
   <si>
-    <t>asdasd</t>
+    <t>cada 1 km</t>
   </si>
 </sst>
 </file>
@@ -382,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +396,7 @@
     <col min="7" max="7" width="11.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +409,11 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -437,8 +441,20 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -463,8 +479,22 @@
         <f>D3/10000</f>
         <v>1.1070000000000001E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
+        <f>SUM(C3:C12)</f>
+        <v>10413.32</v>
+      </c>
+      <c r="N3">
+        <f>SUM(D3:D12)</f>
+        <v>22.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -489,8 +519,22 @@
         <f t="shared" ref="J4:J45" si="2">D4/10000</f>
         <v>1.1070000000000001E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>2000</v>
+      </c>
+      <c r="M4">
+        <f>SUM(C13:C22)</f>
+        <v>8691.5300000000007</v>
+      </c>
+      <c r="N4">
+        <f>SUM(D13:D22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>200</v>
       </c>
@@ -512,8 +556,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>2000</v>
+      </c>
+      <c r="L5">
+        <v>3000</v>
+      </c>
+      <c r="M5">
+        <f>SUM(C23:C32)</f>
+        <v>9406.2900000000009</v>
+      </c>
+      <c r="N5">
+        <f>SUM(D23:D32)</f>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>300</v>
       </c>
@@ -541,8 +599,22 @@
         <f t="shared" si="2"/>
         <v>1.3000000000000001E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>3000</v>
+      </c>
+      <c r="L6">
+        <v>4000</v>
+      </c>
+      <c r="M6">
+        <f>SUM(C33:C42)</f>
+        <v>13749.679999999998</v>
+      </c>
+      <c r="N6">
+        <f>SUM(D33:D42)</f>
+        <v>11.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>400</v>
       </c>
@@ -575,8 +647,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>4000</v>
+      </c>
+      <c r="L7">
+        <v>4300</v>
+      </c>
+      <c r="M7">
+        <f>SUM(C43:C45)</f>
+        <v>2677.32</v>
+      </c>
+      <c r="N7">
+        <f>SUM(D43:D45)</f>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>500</v>
       </c>
@@ -609,8 +695,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f>SUM(M3:M7)</f>
+        <v>44938.14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>600</v>
       </c>
@@ -644,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>700</v>
       </c>
@@ -678,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>800</v>
       </c>
@@ -712,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>900</v>
       </c>
@@ -746,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1000</v>
       </c>
@@ -780,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1100</v>
       </c>
@@ -814,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1200</v>
       </c>
@@ -848,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1300</v>
       </c>
@@ -1840,11 +1930,6 @@
       <c r="D46">
         <f>SUM(D3:D45)</f>
         <v>34.26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglos de los precios unitarios
</commit_message>
<xml_diff>
--- a/corte relleno.xlsx
+++ b/corte relleno.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -386,7 +385,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,6 +697,10 @@
       <c r="M8">
         <f>SUM(M3:M7)</f>
         <v>44938.14</v>
+      </c>
+      <c r="N8">
+        <f>SUM(N3:N7)</f>
+        <v>34.26</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>